<commit_message>
Report + steps loggger is added
updated in selenium
</commit_message>
<xml_diff>
--- a/TestCasesSheet.xlsx
+++ b/TestCasesSheet.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="99">
   <si>
     <t xml:space="preserve">Test cases </t>
   </si>
@@ -121,9 +121,6 @@
     <t>Mrityunjoy</t>
   </si>
   <si>
-    <t xml:space="preserve">Flipkat will be opened </t>
-  </si>
-  <si>
     <t>End Step</t>
   </si>
   <si>
@@ -317,6 +314,15 @@
   </si>
   <si>
     <t>/html/body/div[2]/div/div/div/div/div[2]/div/form/div[3]/button</t>
+  </si>
+  <si>
+    <t>Online Shopping Site for Mobiles, Fashion, Books, Electronics, Home Appliances and More</t>
+  </si>
+  <si>
+    <t>Men's Jackets Online at Best Prices in India - Flipkart.com</t>
+  </si>
+  <si>
+    <t>Fort Collins Full Sleeve Solid Men's Jacket - Buy TAN Fort Collins Full Sleeve Solid Men&amp;#x27;s Jacket Online at Best Prices in India | Flipkart.com</t>
   </si>
 </sst>
 </file>
@@ -791,7 +797,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -800,8 +806,8 @@
     <col min="2" max="2" width="33" style="3" customWidth="1"/>
     <col min="3" max="4" width="15.7109375" style="3" customWidth="1"/>
     <col min="5" max="5" width="21" style="3" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="21.5703125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="38.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" style="4" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" style="3" customWidth="1"/>
     <col min="9" max="9" width="18.140625" style="3" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="3"/>
@@ -818,10 +824,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>25</v>
@@ -842,7 +848,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>22</v>
       </c>
@@ -850,19 +856,19 @@
         <v>21</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>82</v>
-      </c>
       <c r="F2" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>31</v>
+        <v>96</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>11</v>
@@ -871,21 +877,21 @@
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>85</v>
-      </c>
       <c r="G3" s="4" t="s">
-        <v>31</v>
+        <v>96</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>11</v>
@@ -894,21 +900,21 @@
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>87</v>
-      </c>
       <c r="G4" s="4" t="s">
-        <v>31</v>
+        <v>96</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>11</v>
@@ -917,21 +923,21 @@
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>31</v>
+        <v>97</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>11</v>
@@ -940,21 +946,21 @@
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>24</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>31</v>
+        <v>98</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>11</v>
@@ -968,39 +974,37 @@
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+        <v>31</v>
+      </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>82</v>
-      </c>
       <c r="F8" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>31</v>
+        <v>96</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>11</v>
@@ -1009,21 +1013,21 @@
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E9" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>87</v>
-      </c>
       <c r="G9" s="4" t="s">
-        <v>31</v>
+        <v>96</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>11</v>
@@ -1032,21 +1036,21 @@
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>31</v>
+        <v>97</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>11</v>
@@ -1060,19 +1064,17 @@
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+        <v>31</v>
+      </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>26</v>
       </c>
@@ -1080,19 +1082,19 @@
         <v>27</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>82</v>
-      </c>
       <c r="F12" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>31</v>
+        <v>96</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>11</v>
@@ -1101,21 +1103,21 @@
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
     </row>
-    <row r="13" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>28</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>31</v>
+        <v>96</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>11</v>
@@ -1124,21 +1126,21 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>29</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>31</v>
+        <v>96</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>30</v>
@@ -1149,21 +1151,21 @@
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>18</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>31</v>
+        <v>96</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>20</v>
@@ -1174,21 +1176,21 @@
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
     </row>
-    <row r="16" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E16" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="G16" s="4" t="s">
         <v>96</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>11</v>
@@ -1202,13 +1204,11 @@
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
+        <v>31</v>
+      </c>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
@@ -1241,57 +1241,57 @@
   <sheetData>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
         <v>33</v>
-      </c>
-      <c r="C3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
         <v>35</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>36</v>
       </c>
-      <c r="G4" t="s">
-        <v>37</v>
-      </c>
       <c r="H4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" t="s">
         <v>41</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>42</v>
-      </c>
-      <c r="K6" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>21</v>
@@ -1299,169 +1299,169 @@
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="G10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="G11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I12" t="s">
+        <v>40</v>
+      </c>
+      <c r="J12" t="s">
         <v>41</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>42</v>
-      </c>
-      <c r="K12" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" t="s">
         <v>48</v>
       </c>
-      <c r="C14" t="s">
-        <v>49</v>
-      </c>
       <c r="D14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" t="s">
         <v>41</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>42</v>
-      </c>
-      <c r="H15" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" t="s">
         <v>64</v>
-      </c>
-      <c r="B28" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" t="s">
         <v>50</v>
-      </c>
-      <c r="C29" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" t="s">
         <v>52</v>
-      </c>
-      <c r="D30" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E32" t="s">
         <v>25</v>
@@ -1469,74 +1469,74 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E35" t="s">
+        <v>56</v>
+      </c>
+      <c r="F35" t="s">
         <v>57</v>
-      </c>
-      <c r="F35" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F36" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C37" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F37" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
+        <v>60</v>
+      </c>
+      <c r="C38" t="s">
         <v>61</v>
       </c>
-      <c r="C38" t="s">
-        <v>62</v>
-      </c>
       <c r="F38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C39" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C40" t="s">
         <v>3</v>
       </c>
       <c r="D40" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="1048576" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F1048576" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>